<commit_message>
Fix metadata for Frankfurt Melanoma
</commit_message>
<xml_diff>
--- a/Frankfurt_Melanoma/metadata/plate_layout_v1.0.xlsx
+++ b/Frankfurt_Melanoma/metadata/plate_layout_v1.0.xlsx
@@ -73,137 +73,487 @@
   </si>
   <si>
     <t>patient_sample
+Staurosporine
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Staurosporine
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Abemaciclib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Dabrafenib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Capivasertib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Avutometinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Cobimetinib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Vemurafenib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+DMSO
+ 10</t>
+  </si>
+  <si>
+    <t>patient_sample
+Alpelisib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+DMSO
+ 12</t>
+  </si>
+  <si>
+    <t>patient_sample
+Carboplatin
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Vemurafenib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+DMSO
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Alpelisib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Temozolomide
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Vemurafenib + Cobimetinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Alpelisib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Dasatinib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Dacarbazine
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Olaparib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Dabrafenib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Sorafenib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Ulixertinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Dabrafenib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Fluorouracil
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Gemcitabine
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Crizotinib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Everolimus
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Tovorafenib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+DMSO
+ 8</t>
+  </si>
+  <si>
+    <t>patient_sample
+Cediranib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Sorafenib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Temozolomide
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Dasatinib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Cobimetinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Trametinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Carboplatin + Paclitaxel
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Erlotinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+DMSO
+ 5</t>
+  </si>
+  <si>
+    <t>patient_sample
+Neratinib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Fluorouracil
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Carboplatin
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Avutometinib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Capivasertib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Ulixertinib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Trametinib + Erlotinib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Everolimus
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Dabrafenib + Trametinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Cediranib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Trametinib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Vemurafenib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+DMSO
+ 6</t>
+  </si>
+  <si>
+    <t>patient_sample
+Olaparib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Dabrafenib + Trametinib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Carboplatin
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Carboplatin + Paclitaxel
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Gemcitabine
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Carboplatin + Paclitaxel
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Trametinib + Erlotinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Gemcitabine
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Neratinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Everolimus
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Staurosporine
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Erlotinib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+DMSO
+ 7</t>
+  </si>
+  <si>
+    <t>patient_sample
+Crizotinib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Vemurafenib + Cobimetinib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Fluorouracil
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Cobimetinib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Avutometinib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Tovorafenib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Temozolomide
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Dacarbazine
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+DMSO
+ 4</t>
+  </si>
+  <si>
+    <t>patient_sample
+Dasatinib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Trametinib + Erlotinib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Erlotinib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Cediranib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Paclitaxel
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Abemaciclib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Ribociclib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Dacarbazine
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Paclitaxel
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+DMSO
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Capivasertib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Ulixertinib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Ribociclib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Sorafenib
+ 1</t>
+  </si>
+  <si>
+    <t>patient_sample
+Ribociclib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+Abemaciclib
+ 2</t>
+  </si>
+  <si>
+    <t>patient_sample
+DMSO
+ 9</t>
+  </si>
+  <si>
+    <t>patient_sample
+Trametinib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Olaparib
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
+Paclitaxel
+ 3</t>
+  </si>
+  <si>
+    <t>patient_sample
 Crizotinib
  1</t>
   </si>
   <si>
     <t>patient_sample
-Avutometinib
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Sorafenib
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Trametinib
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Sorafenib
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Ulixertinib
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Ribociclib
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Paclitaxel
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-DMSO
- 10</t>
-  </si>
-  <si>
-    <t>patient_sample
-Flouroracil
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-DMSO
- 12</t>
-  </si>
-  <si>
-    <t>patient_sample
-Dabrafenib
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Trametinib
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-DMSO
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Everolimus
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Trametinib + Erlotinib
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Neratinib
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Cobimetinib
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Neratinib
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Alpelisib
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Dabrafenib
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Cobimetinib
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Avutometinib
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Olaparib
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Sorafenib
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Dabrafenib + Trametinib
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Trametinib
+Tovorafenib
  2</t>
   </si>
   <si>
@@ -213,366 +563,16 @@
   </si>
   <si>
     <t>patient_sample
-Flouroracil
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Cediranib
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-DMSO
- 8</t>
-  </si>
-  <si>
-    <t>patient_sample
-Everolimus
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
 Vemurafenib + Cobimetinib
  2</t>
   </si>
   <si>
     <t>patient_sample
-Cediranib
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Olaparib
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Abemaciclib
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Ribociclib
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Erlotinib
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Tovorafenib
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-DMSO
- 5</t>
-  </si>
-  <si>
-    <t>patient_sample
-Dacarbazine
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Everolimus
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Carboplatin
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Trametinib + Erlotinib
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Staurosporine
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Vemurafenib + Cobimetinib
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Gemcitabine
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Vemurafenib
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Trametinib + Erlotinib
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Cobimetinib
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Olaparib
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Gemcitabine
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-DMSO
- 6</t>
-  </si>
-  <si>
-    <t>patient_sample
-Flouroracil
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Capivasertib
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Tovorafenib
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Dasatinib
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Dabrafenib
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Dasatinib
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Carboplatin
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Capivasertib
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Dasatinib
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Staurosporine
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Crizotinib
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Vemurafenib + Cobimetinib
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-DMSO
- 7</t>
-  </si>
-  <si>
-    <t>patient_sample
-Paclitaxel
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Abemaciclib
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Carboplatin
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Abemaciclib
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Capivasertib
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Alpelisib
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Staurosporine
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Vemurafenib
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-DMSO
- 4</t>
-  </si>
-  <si>
-    <t>patient_sample
-Alpelisib
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Cediranib
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Gemcitabine
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Avutometinib
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Temozolomide
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Crizotinib
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Dabrafenib + Trametinib
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
 Neratinib
  3</t>
   </si>
   <si>
     <t>patient_sample
-Paclitaxel
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-DMSO
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Temozolomide
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Dacarbazine
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Ulixertinib
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Temozolomide
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Erlotinib
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Carboplatin + Paclitaxel
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-DMSO
- 9</t>
-  </si>
-  <si>
-    <t>patient_sample
-Erlotinib
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Tovorafenib
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Ribociclib
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Ulixertinib
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Carboplatin + Paclitaxel
- 1</t>
-  </si>
-  <si>
-    <t>patient_sample
-Carboplatin + Paclitaxel
- 2</t>
-  </si>
-  <si>
-    <t>patient_sample
-Dacarbazine
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
-Vemurafenib
- 3</t>
-  </si>
-  <si>
-    <t>patient_sample
 DMSO
  11</t>
   </si>
@@ -583,94 +583,94 @@
     <t>DMSO</t>
   </si>
   <si>
+    <t>Staurosporine</t>
+  </si>
+  <si>
+    <t>Abemaciclib</t>
+  </si>
+  <si>
+    <t>Dabrafenib</t>
+  </si>
+  <si>
+    <t>Capivasertib</t>
+  </si>
+  <si>
+    <t>Avutometinib</t>
+  </si>
+  <si>
+    <t>Cobimetinib</t>
+  </si>
+  <si>
+    <t>Vemurafenib</t>
+  </si>
+  <si>
+    <t>Alpelisib</t>
+  </si>
+  <si>
+    <t>Carboplatin</t>
+  </si>
+  <si>
+    <t>Temozolomide</t>
+  </si>
+  <si>
+    <t>Vemurafenib + Cobimetinib</t>
+  </si>
+  <si>
+    <t>Dasatinib</t>
+  </si>
+  <si>
+    <t>Dacarbazine</t>
+  </si>
+  <si>
+    <t>Olaparib</t>
+  </si>
+  <si>
+    <t>Sorafenib</t>
+  </si>
+  <si>
+    <t>Ulixertinib</t>
+  </si>
+  <si>
+    <t>Fluorouracil</t>
+  </si>
+  <si>
+    <t>Gemcitabine</t>
+  </si>
+  <si>
     <t>Crizotinib</t>
   </si>
   <si>
-    <t>Avutometinib</t>
-  </si>
-  <si>
-    <t>Sorafenib</t>
+    <t>Everolimus</t>
+  </si>
+  <si>
+    <t>Tovorafenib</t>
+  </si>
+  <si>
+    <t>Cediranib</t>
   </si>
   <si>
     <t>Trametinib</t>
   </si>
   <si>
-    <t>Ulixertinib</t>
+    <t>Carboplatin + Paclitaxel</t>
+  </si>
+  <si>
+    <t>Erlotinib</t>
+  </si>
+  <si>
+    <t>Neratinib</t>
+  </si>
+  <si>
+    <t>Trametinib + Erlotinib</t>
+  </si>
+  <si>
+    <t>Dabrafenib + Trametinib</t>
+  </si>
+  <si>
+    <t>Paclitaxel</t>
   </si>
   <si>
     <t>Ribociclib</t>
-  </si>
-  <si>
-    <t>Paclitaxel</t>
-  </si>
-  <si>
-    <t>Flouroracil</t>
-  </si>
-  <si>
-    <t>Dabrafenib</t>
-  </si>
-  <si>
-    <t>Everolimus</t>
-  </si>
-  <si>
-    <t>Trametinib + Erlotinib</t>
-  </si>
-  <si>
-    <t>Neratinib</t>
-  </si>
-  <si>
-    <t>Cobimetinib</t>
-  </si>
-  <si>
-    <t>Alpelisib</t>
-  </si>
-  <si>
-    <t>Olaparib</t>
-  </si>
-  <si>
-    <t>Dabrafenib + Trametinib</t>
-  </si>
-  <si>
-    <t>Cediranib</t>
-  </si>
-  <si>
-    <t>Vemurafenib + Cobimetinib</t>
-  </si>
-  <si>
-    <t>Abemaciclib</t>
-  </si>
-  <si>
-    <t>Erlotinib</t>
-  </si>
-  <si>
-    <t>Tovorafenib</t>
-  </si>
-  <si>
-    <t>Dacarbazine</t>
-  </si>
-  <si>
-    <t>Carboplatin</t>
-  </si>
-  <si>
-    <t>Staurosporine</t>
-  </si>
-  <si>
-    <t>Gemcitabine</t>
-  </si>
-  <si>
-    <t>Vemurafenib</t>
-  </si>
-  <si>
-    <t>Capivasertib</t>
-  </si>
-  <si>
-    <t>Dasatinib</t>
-  </si>
-  <si>
-    <t>Temozolomide</t>
-  </si>
-  <si>
-    <t>Carboplatin + Paclitaxel</t>
   </si>
   <si>
     <t>1</t>
@@ -2198,25 +2198,25 @@
         <v>128</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="60" customHeight="1">
@@ -2227,22 +2227,22 @@
         <v>120</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>122</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>119</v>
@@ -2253,31 +2253,31 @@
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>119</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="K6" s="1" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="60" customHeight="1">
@@ -2285,28 +2285,28 @@
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>119</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="60" customHeight="1">
@@ -2314,31 +2314,31 @@
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>119</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>120</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="60" customHeight="1">
@@ -2346,28 +2346,28 @@
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>119</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="60" customHeight="1">
@@ -2378,16 +2378,16 @@
         <v>124</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="H10" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>119</v>
@@ -2396,10 +2396,10 @@
         <v>144</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="60" customHeight="1">
@@ -2416,19 +2416,19 @@
         <v>119</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="J11" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="60" customHeight="1">
@@ -2439,19 +2439,19 @@
         <v>126</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>148</v>
@@ -2471,25 +2471,25 @@
         <v>119</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="I13" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="60" customHeight="1">
@@ -2500,25 +2500,25 @@
         <v>127</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="I14" s="1" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>119</v>
@@ -2532,25 +2532,25 @@
         <v>119</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="60" customHeight="1">
@@ -2744,7 +2744,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>152</v>
@@ -2762,13 +2762,13 @@
         <v>150</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>150</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="60" customHeight="1">
@@ -2776,7 +2776,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>150</v>
@@ -2797,7 +2797,7 @@
         <v>159</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="60" customHeight="1">
@@ -2805,7 +2805,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>151</v>
@@ -2817,16 +2817,16 @@
         <v>156</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="K8" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>151</v>
@@ -2837,13 +2837,13 @@
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>150</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>151</v>
@@ -2852,13 +2852,13 @@
         <v>157</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="60" customHeight="1">
@@ -2866,31 +2866,31 @@
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>151</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>151</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>158</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>151</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="60" customHeight="1">
@@ -2910,16 +2910,16 @@
         <v>151</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>151</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="60" customHeight="1">
@@ -2930,22 +2930,22 @@
         <v>152</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>152</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>160</v>

</xml_diff>